<commit_message>
Share Skill & Manage Listings
</commit_message>
<xml_diff>
--- a/Mars_Ava.xlsx
+++ b/Mars_Ava.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299">
   <si>
     <t xml:space="preserve">Test Condition ID </t>
   </si>
@@ -791,7 +791,7 @@
     <t>Seller should be able to see no red error message</t>
   </si>
   <si>
-    <t>Seller should be able to see the popup message "Service Listing Added Successfully."</t>
+    <t>Seller should be able to see the popup message "Service Listing Added successfully."</t>
   </si>
   <si>
     <t>TC_015_01</t>
@@ -897,6 +897,12 @@
   </si>
   <si>
     <t>TC_022_01</t>
+  </si>
+  <si>
+    <t>Step 4: Select the second page</t>
+  </si>
+  <si>
+    <t>Seller should be able to see the second page with all service listings</t>
   </si>
   <si>
     <t>Step 5: Click on the icon of the previous page</t>
@@ -920,9 +926,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -953,24 +959,54 @@
       <charset val="134"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -983,45 +1019,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1030,8 +1027,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1053,14 +1058,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1082,8 +1080,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1092,6 +1091,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1112,55 +1118,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1172,31 +1154,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1214,7 +1172,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1226,19 +1184,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1250,49 +1292,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1307,16 +1313,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1345,21 +1351,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1369,11 +1360,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1403,10 +1400,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1424,134 +1430,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1564,17 +1570,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1585,9 +1585,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1595,9 +1592,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1873,7 +1867,7 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" outlineLevelCol="6"/>
@@ -1894,125 +1888,125 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:4">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:4">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:4">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:4">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:7">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:4">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:4">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:4">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:4">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:4">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:4">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:4">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2020,43 +2014,43 @@
       </c>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:4">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:4">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:4">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" spans="1:4">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" spans="1:4">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -2064,151 +2058,151 @@
       </c>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:4">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="1" spans="1:4">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" spans="1:4">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12" t="s">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:4">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" spans="1:4">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="1" spans="1:4">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12" t="s">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" spans="1:4">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12" t="s">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" spans="1:4">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12" t="s">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" spans="1:4">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12" t="s">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" spans="1:4">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12" t="s">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" spans="1:4">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12" t="s">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" spans="1:4">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12" t="s">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" spans="1:4">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12" t="s">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" spans="1:4">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12" t="s">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="1" spans="1:4">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="1" spans="1:4">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12" t="s">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" spans="1:4">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -2216,280 +2210,280 @@
       </c>
     </row>
     <row r="36" s="1" customFormat="1" spans="1:4">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
       <c r="D36" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" spans="1:4">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="1" spans="1:4">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
       <c r="D38" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" spans="1:4">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
       <c r="D39" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" s="1" customFormat="1" spans="1:4">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" s="1" customFormat="1" spans="1:4">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12" t="s">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42" s="1" customFormat="1" spans="1:4">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12" t="s">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="43" s="1" customFormat="1" spans="1:4">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12" t="s">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="44" s="1" customFormat="1" spans="1:4">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
       <c r="D44" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="45" s="1" customFormat="1" spans="1:4">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12" t="s">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" spans="1:4">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12" t="s">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="1" spans="1:4">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12" t="s">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="1" spans="1:4">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12" t="s">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="49" s="1" customFormat="1" spans="1:4">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="12"/>
-      <c r="C49" s="14" t="s">
+      <c r="B49" s="4"/>
+      <c r="C49" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" spans="1:4">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="51" s="1" customFormat="1" spans="1:4">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="16" t="s">
+      <c r="B51" s="4"/>
+      <c r="C51" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="52" s="1" customFormat="1" spans="1:4">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="12" t="s">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="53" s="1" customFormat="1" spans="1:4">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B53" s="12"/>
-      <c r="C53" s="15" t="s">
+      <c r="B53" s="4"/>
+      <c r="C53" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="54" s="1" customFormat="1" spans="1:4">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="12"/>
-      <c r="C54" s="15" t="s">
+      <c r="B54" s="4"/>
+      <c r="C54" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="55" s="1" customFormat="1" spans="1:4">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="16" t="s">
+      <c r="B55" s="4"/>
+      <c r="C55" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="1" spans="1:4">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="12" t="s">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="1" spans="1:4">
-      <c r="A57" s="12" t="s">
+      <c r="A57" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12" t="s">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="1" spans="1:4">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12" t="s">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="1" spans="1:4">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12" t="s">
+      <c r="B59" s="4"/>
+      <c r="C59" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="4" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="60" s="1" customFormat="1" spans="1:4">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
     </row>
     <row r="61" s="1" customFormat="1" spans="1:4">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
     </row>
     <row r="62" s="1" customFormat="1" spans="1:4">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
     </row>
     <row r="63" s="1" customFormat="1" spans="1:4">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
     </row>
     <row r="64" s="1" customFormat="1" spans="1:4">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
     </row>
     <row r="65" s="1" customFormat="1"/>
     <row r="66" s="1" customFormat="1"/>
@@ -2546,8 +2540,8 @@
   <sheetPr/>
   <dimension ref="A1:G275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
-      <selection activeCell="A252" sqref="A252:A255"/>
+    <sheetView tabSelected="1" topLeftCell="D193" workbookViewId="0">
+      <selection activeCell="D201" sqref="D201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -2595,17 +2589,17 @@
       <c r="C2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="63" spans="1:4">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2615,12 +2609,12 @@
       <c r="C4" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B5" s="4" t="str">
@@ -2630,32 +2624,32 @@
       <c r="C5" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>115</v>
@@ -2665,7 +2659,7 @@
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B9" s="4" t="str">
@@ -2675,33 +2669,33 @@
       <c r="C9" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A12" s="8"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
         <v>118</v>
       </c>
@@ -2710,7 +2704,7 @@
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B13" s="4" t="str">
@@ -2720,42 +2714,42 @@
       <c r="C13" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A16" s="8"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>123</v>
       </c>
       <c r="B17" s="4" t="str">
@@ -2765,42 +2759,42 @@
       <c r="C17" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="1" ht="42" spans="1:4">
-      <c r="A20" s="8"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>126</v>
       </c>
       <c r="B21" s="4" t="str">
@@ -2810,33 +2804,33 @@
       <c r="C21" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A23" s="7"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A24" s="8"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>127</v>
       </c>
@@ -2845,7 +2839,7 @@
       </c>
     </row>
     <row r="25" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>128</v>
       </c>
       <c r="B25" s="4" t="str">
@@ -2855,33 +2849,33 @@
       <c r="C25" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A26" s="7"/>
+      <c r="A26" s="6"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="5" t="s">
+      <c r="C26" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A27" s="7"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A28" s="8"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
         <v>129</v>
       </c>
@@ -2890,7 +2884,7 @@
       </c>
     </row>
     <row r="29" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>130</v>
       </c>
       <c r="B29" s="4" t="str">
@@ -2900,42 +2894,42 @@
       <c r="C29" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A30" s="7"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A31" s="7"/>
+      <c r="A31" s="6"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A32" s="8"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="7" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>132</v>
       </c>
       <c r="B33" s="4" t="str">
@@ -2945,42 +2939,42 @@
       <c r="C33" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A34" s="7"/>
+      <c r="A34" s="6"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="5" t="s">
+      <c r="C34" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A35" s="7"/>
+      <c r="A35" s="6"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="1" ht="42" spans="1:4">
-      <c r="A36" s="8"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="7" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>135</v>
       </c>
       <c r="B37" s="4" t="str">
@@ -2990,33 +2984,33 @@
       <c r="C37" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A38" s="7"/>
+      <c r="A38" s="6"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="5" t="s">
+      <c r="C38" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A39" s="7"/>
+      <c r="A39" s="6"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="40" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A40" s="8"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
         <v>136</v>
       </c>
@@ -3025,7 +3019,7 @@
       </c>
     </row>
     <row r="41" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>138</v>
       </c>
       <c r="B41" s="4" t="str">
@@ -3035,33 +3029,33 @@
       <c r="C41" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="42" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A42" s="7"/>
+      <c r="A42" s="6"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="C42" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="43" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A43" s="7"/>
+      <c r="A43" s="6"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="44" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A44" s="8"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
         <v>139</v>
       </c>
@@ -3070,7 +3064,7 @@
       </c>
     </row>
     <row r="45" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>141</v>
       </c>
       <c r="B45" s="4" t="str">
@@ -3080,32 +3074,32 @@
       <c r="C45" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A46" s="7"/>
+      <c r="A46" s="6"/>
       <c r="B46" s="4"/>
-      <c r="C46" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D46" s="5" t="s">
+      <c r="C46" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A47" s="7"/>
+      <c r="A47" s="6"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A48" s="7"/>
+      <c r="A48" s="6"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4" t="s">
         <v>142</v>
@@ -3115,8 +3109,8 @@
       </c>
     </row>
     <row r="49" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A49" s="8"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
         <v>144</v>
       </c>
@@ -3125,7 +3119,7 @@
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B50" s="4" t="str">
@@ -3135,32 +3129,32 @@
       <c r="C50" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="51" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A51" s="7"/>
+      <c r="A51" s="6"/>
       <c r="B51" s="4"/>
-      <c r="C51" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D51" s="5" t="s">
+      <c r="C51" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="52" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A52" s="7"/>
+      <c r="A52" s="6"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="53" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A53" s="7"/>
+      <c r="A53" s="6"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4" t="s">
         <v>147</v>
@@ -3170,8 +3164,8 @@
       </c>
     </row>
     <row r="54" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A54" s="8"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="6"/>
+      <c r="B54" s="4"/>
       <c r="C54" s="4" t="s">
         <v>144</v>
       </c>
@@ -3180,7 +3174,7 @@
       </c>
     </row>
     <row r="55" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
         <v>150</v>
       </c>
       <c r="B55" s="4" t="str">
@@ -3190,32 +3184,32 @@
       <c r="C55" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A56" s="7"/>
+      <c r="A56" s="6"/>
       <c r="B56" s="4"/>
-      <c r="C56" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D56" s="5" t="s">
+      <c r="C56" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A57" s="7"/>
+      <c r="A57" s="6"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A58" s="7"/>
+      <c r="A58" s="6"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4" t="s">
         <v>151</v>
@@ -3225,8 +3219,8 @@
       </c>
     </row>
     <row r="59" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A59" s="8"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="6"/>
+      <c r="B59" s="4"/>
       <c r="C59" s="4" t="s">
         <v>144</v>
       </c>
@@ -3235,7 +3229,7 @@
       </c>
     </row>
     <row r="60" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="6" t="s">
         <v>154</v>
       </c>
       <c r="B60" s="4" t="str">
@@ -3245,32 +3239,32 @@
       <c r="C60" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A61" s="7"/>
+      <c r="A61" s="6"/>
       <c r="B61" s="4"/>
-      <c r="C61" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D61" s="5" t="s">
+      <c r="C61" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A62" s="7"/>
+      <c r="A62" s="6"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="63" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A63" s="7"/>
+      <c r="A63" s="6"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4" t="s">
         <v>155</v>
@@ -3280,8 +3274,8 @@
       </c>
     </row>
     <row r="64" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A64" s="8"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
         <v>144</v>
       </c>
@@ -3290,7 +3284,7 @@
       </c>
     </row>
     <row r="65" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B65" s="4" t="str">
@@ -3300,32 +3294,32 @@
       <c r="C65" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="66" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A66" s="7"/>
+      <c r="A66" s="6"/>
       <c r="B66" s="4"/>
-      <c r="C66" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D66" s="5" t="s">
+      <c r="C66" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A67" s="7"/>
+      <c r="A67" s="6"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="68" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A68" s="7"/>
+      <c r="A68" s="6"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
         <v>159</v>
@@ -3335,8 +3329,8 @@
       </c>
     </row>
     <row r="69" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A69" s="8"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="6"/>
+      <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
         <v>144</v>
       </c>
@@ -3345,7 +3339,7 @@
       </c>
     </row>
     <row r="70" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="6" t="s">
         <v>162</v>
       </c>
       <c r="B70" s="4" t="str">
@@ -3355,33 +3349,33 @@
       <c r="C70" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="71" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A71" s="7"/>
+      <c r="A71" s="6"/>
       <c r="B71" s="4"/>
-      <c r="C71" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D71" s="5" t="s">
+      <c r="C71" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D71" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="72" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A72" s="7"/>
+      <c r="A72" s="6"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="73" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A73" s="8"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="6"/>
+      <c r="B73" s="4"/>
       <c r="C73" s="4" t="s">
         <v>163</v>
       </c>
@@ -3390,7 +3384,7 @@
       </c>
     </row>
     <row r="74" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="6" t="s">
         <v>165</v>
       </c>
       <c r="B74" s="4" t="str">
@@ -3400,33 +3394,33 @@
       <c r="C74" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A75" s="7"/>
+      <c r="A75" s="6"/>
       <c r="B75" s="4"/>
-      <c r="C75" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D75" s="5" t="s">
+      <c r="C75" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="76" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A76" s="7"/>
+      <c r="A76" s="6"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="77" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A77" s="8"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="6"/>
+      <c r="B77" s="4"/>
       <c r="C77" s="4" t="s">
         <v>166</v>
       </c>
@@ -3435,7 +3429,7 @@
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="6" t="s">
         <v>168</v>
       </c>
       <c r="B78" s="4" t="str">
@@ -3445,33 +3439,33 @@
       <c r="C78" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="79" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A79" s="7"/>
+      <c r="A79" s="6"/>
       <c r="B79" s="4"/>
-      <c r="C79" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D79" s="5" t="s">
+      <c r="C79" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D79" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="80" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A80" s="7"/>
+      <c r="A80" s="6"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="81" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A81" s="8"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="6"/>
+      <c r="B81" s="4"/>
       <c r="C81" s="4" t="s">
         <v>169</v>
       </c>
@@ -3480,7 +3474,7 @@
       </c>
     </row>
     <row r="82" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="6" t="s">
         <v>171</v>
       </c>
       <c r="B82" s="4" t="str">
@@ -3490,33 +3484,33 @@
       <c r="C82" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="83" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A83" s="7"/>
+      <c r="A83" s="6"/>
       <c r="B83" s="4"/>
-      <c r="C83" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D83" s="5" t="s">
+      <c r="C83" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D83" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="84" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A84" s="7"/>
+      <c r="A84" s="6"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A85" s="8"/>
-      <c r="B85" s="5"/>
+      <c r="A85" s="6"/>
+      <c r="B85" s="4"/>
       <c r="C85" s="4" t="s">
         <v>172</v>
       </c>
@@ -3525,7 +3519,7 @@
       </c>
     </row>
     <row r="86" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="6" t="s">
         <v>174</v>
       </c>
       <c r="B86" s="4" t="str">
@@ -3535,32 +3529,32 @@
       <c r="C86" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A87" s="7"/>
+      <c r="A87" s="6"/>
       <c r="B87" s="4"/>
-      <c r="C87" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D87" s="5" t="s">
+      <c r="C87" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="88" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A88" s="7"/>
+      <c r="A88" s="6"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="89" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A89" s="8"/>
+      <c r="A89" s="6"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4" t="s">
         <v>175</v>
@@ -3570,7 +3564,7 @@
       </c>
     </row>
     <row r="90" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="6" t="s">
         <v>177</v>
       </c>
       <c r="B90" s="4" t="str">
@@ -3580,33 +3574,33 @@
       <c r="C90" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="91" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A91" s="7"/>
+      <c r="A91" s="6"/>
       <c r="B91" s="4"/>
-      <c r="C91" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D91" s="5" t="s">
+      <c r="C91" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="92" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A92" s="7"/>
+      <c r="A92" s="6"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D92" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A93" s="8"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="6"/>
+      <c r="B93" s="4"/>
       <c r="C93" s="4" t="s">
         <v>178</v>
       </c>
@@ -3615,7 +3609,7 @@
       </c>
     </row>
     <row r="94" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="6" t="s">
         <v>180</v>
       </c>
       <c r="B94" s="4" t="str">
@@ -3625,33 +3619,33 @@
       <c r="C94" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="95" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A95" s="7"/>
+      <c r="A95" s="6"/>
       <c r="B95" s="4"/>
-      <c r="C95" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D95" s="5" t="s">
+      <c r="C95" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D95" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="96" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A96" s="7"/>
+      <c r="A96" s="6"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="97" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A97" s="8"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="6"/>
+      <c r="B97" s="4"/>
       <c r="C97" s="4" t="s">
         <v>181</v>
       </c>
@@ -3660,7 +3654,7 @@
       </c>
     </row>
     <row r="98" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="6" t="s">
         <v>183</v>
       </c>
       <c r="B98" s="4" t="str">
@@ -3670,33 +3664,33 @@
       <c r="C98" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A99" s="7"/>
+      <c r="A99" s="6"/>
       <c r="B99" s="4"/>
-      <c r="C99" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D99" s="5" t="s">
+      <c r="C99" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D99" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A100" s="7"/>
+      <c r="A100" s="6"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A101" s="8"/>
-      <c r="B101" s="5"/>
+      <c r="A101" s="6"/>
+      <c r="B101" s="4"/>
       <c r="C101" s="4" t="s">
         <v>184</v>
       </c>
@@ -3705,7 +3699,7 @@
       </c>
     </row>
     <row r="102" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A102" s="7" t="s">
+      <c r="A102" s="6" t="s">
         <v>186</v>
       </c>
       <c r="B102" s="4" t="str">
@@ -3715,33 +3709,33 @@
       <c r="C102" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="103" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A103" s="7"/>
+      <c r="A103" s="6"/>
       <c r="B103" s="4"/>
-      <c r="C103" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D103" s="5" t="s">
+      <c r="C103" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D103" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A104" s="7"/>
+      <c r="A104" s="6"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D104" s="5" t="s">
+      <c r="D104" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A105" s="8"/>
-      <c r="B105" s="5"/>
+      <c r="A105" s="6"/>
+      <c r="B105" s="4"/>
       <c r="C105" s="4" t="s">
         <v>187</v>
       </c>
@@ -3750,7 +3744,7 @@
       </c>
     </row>
     <row r="106" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A106" s="7" t="s">
+      <c r="A106" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B106" s="4" t="str">
@@ -3760,33 +3754,33 @@
       <c r="C106" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="D106" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A107" s="7"/>
+      <c r="A107" s="6"/>
       <c r="B107" s="4"/>
-      <c r="C107" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D107" s="5" t="s">
+      <c r="C107" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D107" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A108" s="7"/>
+      <c r="A108" s="6"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D108" s="5" t="s">
+      <c r="D108" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A109" s="8"/>
-      <c r="B109" s="5"/>
+      <c r="A109" s="6"/>
+      <c r="B109" s="4"/>
       <c r="C109" s="4" t="s">
         <v>190</v>
       </c>
@@ -3795,7 +3789,7 @@
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A110" s="7" t="s">
+      <c r="A110" s="6" t="s">
         <v>192</v>
       </c>
       <c r="B110" s="4" t="str">
@@ -3805,32 +3799,32 @@
       <c r="C110" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D110" s="5" t="s">
+      <c r="D110" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A111" s="7"/>
+      <c r="A111" s="6"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D111" s="5" t="s">
+      <c r="C111" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D111" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A112" s="7"/>
+      <c r="A112" s="6"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="D112" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A113" s="7"/>
+      <c r="A113" s="6"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4" t="s">
         <v>193</v>
@@ -3840,8 +3834,8 @@
       </c>
     </row>
     <row r="114" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A114" s="8"/>
-      <c r="B114" s="5"/>
+      <c r="A114" s="6"/>
+      <c r="B114" s="4"/>
       <c r="C114" s="4" t="s">
         <v>195</v>
       </c>
@@ -3850,7 +3844,7 @@
       </c>
     </row>
     <row r="115" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A115" s="7" t="s">
+      <c r="A115" s="6" t="s">
         <v>197</v>
       </c>
       <c r="B115" s="4" t="str">
@@ -3860,33 +3854,33 @@
       <c r="C115" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="D115" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="116" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A116" s="7"/>
+      <c r="A116" s="6"/>
       <c r="B116" s="4"/>
-      <c r="C116" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D116" s="5" t="s">
+      <c r="C116" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D116" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A117" s="7"/>
+      <c r="A117" s="6"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="D117" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A118" s="8"/>
-      <c r="B118" s="5"/>
+      <c r="A118" s="6"/>
+      <c r="B118" s="4"/>
       <c r="C118" s="4" t="s">
         <v>198</v>
       </c>
@@ -3895,7 +3889,7 @@
       </c>
     </row>
     <row r="119" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A119" s="7" t="s">
+      <c r="A119" s="6" t="s">
         <v>200</v>
       </c>
       <c r="B119" s="4" t="str">
@@ -3905,33 +3899,33 @@
       <c r="C119" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D119" s="5" t="s">
+      <c r="D119" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A120" s="7"/>
+      <c r="A120" s="6"/>
       <c r="B120" s="4"/>
-      <c r="C120" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D120" s="5" t="s">
+      <c r="C120" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D120" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="121" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A121" s="7"/>
+      <c r="A121" s="6"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D121" s="5" t="s">
+      <c r="D121" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A122" s="8"/>
-      <c r="B122" s="5"/>
+      <c r="A122" s="6"/>
+      <c r="B122" s="4"/>
       <c r="C122" s="4" t="s">
         <v>198</v>
       </c>
@@ -3940,7 +3934,7 @@
       </c>
     </row>
     <row r="123" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A123" s="7" t="s">
+      <c r="A123" s="6" t="s">
         <v>202</v>
       </c>
       <c r="B123" s="4" t="str">
@@ -3950,33 +3944,33 @@
       <c r="C123" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D123" s="5" t="s">
+      <c r="D123" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="124" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A124" s="7"/>
+      <c r="A124" s="6"/>
       <c r="B124" s="4"/>
-      <c r="C124" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D124" s="5" t="s">
+      <c r="C124" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D124" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A125" s="7"/>
+      <c r="A125" s="6"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D125" s="5" t="s">
+      <c r="D125" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A126" s="8"/>
-      <c r="B126" s="5"/>
+      <c r="A126" s="6"/>
+      <c r="B126" s="4"/>
       <c r="C126" s="4" t="s">
         <v>203</v>
       </c>
@@ -3985,7 +3979,7 @@
       </c>
     </row>
     <row r="127" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A127" s="7" t="s">
+      <c r="A127" s="6" t="s">
         <v>205</v>
       </c>
       <c r="B127" s="4" t="str">
@@ -3995,33 +3989,33 @@
       <c r="C127" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D127" s="5" t="s">
+      <c r="D127" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A128" s="7"/>
+      <c r="A128" s="6"/>
       <c r="B128" s="4"/>
-      <c r="C128" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D128" s="5" t="s">
+      <c r="C128" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D128" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A129" s="7"/>
+      <c r="A129" s="6"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D129" s="5" t="s">
+      <c r="D129" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A130" s="8"/>
-      <c r="B130" s="5"/>
+      <c r="A130" s="6"/>
+      <c r="B130" s="4"/>
       <c r="C130" s="4" t="s">
         <v>206</v>
       </c>
@@ -4030,7 +4024,7 @@
       </c>
     </row>
     <row r="131" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A131" s="7" t="s">
+      <c r="A131" s="6" t="s">
         <v>208</v>
       </c>
       <c r="B131" s="4" t="str">
@@ -4040,33 +4034,33 @@
       <c r="C131" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D131" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="132" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A132" s="7"/>
+      <c r="A132" s="6"/>
       <c r="B132" s="4"/>
-      <c r="C132" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D132" s="5" t="s">
+      <c r="C132" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D132" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="133" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A133" s="7"/>
+      <c r="A133" s="6"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D133" s="5" t="s">
+      <c r="D133" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="134" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A134" s="8"/>
-      <c r="B134" s="5"/>
+      <c r="A134" s="6"/>
+      <c r="B134" s="4"/>
       <c r="C134" s="4" t="s">
         <v>209</v>
       </c>
@@ -4075,7 +4069,7 @@
       </c>
     </row>
     <row r="135" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A135" s="7" t="s">
+      <c r="A135" s="6" t="s">
         <v>211</v>
       </c>
       <c r="B135" s="4" t="str">
@@ -4085,33 +4079,33 @@
       <c r="C135" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D135" s="5" t="s">
+      <c r="D135" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A136" s="7"/>
+      <c r="A136" s="6"/>
       <c r="B136" s="4"/>
-      <c r="C136" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D136" s="5" t="s">
+      <c r="C136" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D136" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A137" s="7"/>
+      <c r="A137" s="6"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D137" s="5" t="s">
+      <c r="D137" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A138" s="8"/>
-      <c r="B138" s="5"/>
+      <c r="A138" s="6"/>
+      <c r="B138" s="4"/>
       <c r="C138" s="4" t="s">
         <v>212</v>
       </c>
@@ -4120,7 +4114,7 @@
       </c>
     </row>
     <row r="139" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A139" s="7" t="s">
+      <c r="A139" s="6" t="s">
         <v>214</v>
       </c>
       <c r="B139" s="4" t="str">
@@ -4130,32 +4124,32 @@
       <c r="C139" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D139" s="5" t="s">
+      <c r="D139" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A140" s="7"/>
+      <c r="A140" s="6"/>
       <c r="B140" s="4"/>
-      <c r="C140" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D140" s="5" t="s">
+      <c r="C140" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D140" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A141" s="7"/>
+      <c r="A141" s="6"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D141" s="5" t="s">
+      <c r="D141" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A142" s="7"/>
+      <c r="A142" s="6"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4" t="s">
         <v>215</v>
@@ -4165,8 +4159,8 @@
       </c>
     </row>
     <row r="143" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A143" s="8"/>
-      <c r="B143" s="5"/>
+      <c r="A143" s="6"/>
+      <c r="B143" s="4"/>
       <c r="C143" s="4" t="s">
         <v>144</v>
       </c>
@@ -4175,7 +4169,7 @@
       </c>
     </row>
     <row r="144" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A144" s="7" t="s">
+      <c r="A144" s="6" t="s">
         <v>217</v>
       </c>
       <c r="B144" s="4" t="str">
@@ -4185,32 +4179,32 @@
       <c r="C144" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D144" s="5" t="s">
+      <c r="D144" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A145" s="7"/>
+      <c r="A145" s="6"/>
       <c r="B145" s="4"/>
-      <c r="C145" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D145" s="5" t="s">
+      <c r="C145" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D145" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A146" s="7"/>
+      <c r="A146" s="6"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D146" s="5" t="s">
+      <c r="D146" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A147" s="7"/>
+      <c r="A147" s="6"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4" t="s">
         <v>218</v>
@@ -4220,8 +4214,8 @@
       </c>
     </row>
     <row r="148" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A148" s="8"/>
-      <c r="B148" s="5"/>
+      <c r="A148" s="6"/>
+      <c r="B148" s="4"/>
       <c r="C148" s="4" t="s">
         <v>144</v>
       </c>
@@ -4230,7 +4224,7 @@
       </c>
     </row>
     <row r="149" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A149" s="7" t="s">
+      <c r="A149" s="6" t="s">
         <v>220</v>
       </c>
       <c r="B149" s="4" t="str">
@@ -4240,32 +4234,32 @@
       <c r="C149" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D149" s="5" t="s">
+      <c r="D149" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A150" s="7"/>
+      <c r="A150" s="6"/>
       <c r="B150" s="4"/>
-      <c r="C150" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D150" s="5" t="s">
+      <c r="C150" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D150" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A151" s="7"/>
+      <c r="A151" s="6"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D151" s="5" t="s">
+      <c r="D151" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A152" s="7"/>
+      <c r="A152" s="6"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4" t="s">
         <v>221</v>
@@ -4275,8 +4269,8 @@
       </c>
     </row>
     <row r="153" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A153" s="8"/>
-      <c r="B153" s="5"/>
+      <c r="A153" s="6"/>
+      <c r="B153" s="4"/>
       <c r="C153" s="4" t="s">
         <v>144</v>
       </c>
@@ -4285,7 +4279,7 @@
       </c>
     </row>
     <row r="154" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A154" s="7" t="s">
+      <c r="A154" s="6" t="s">
         <v>223</v>
       </c>
       <c r="B154" s="4" t="str">
@@ -4295,32 +4289,32 @@
       <c r="C154" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D154" s="5" t="s">
+      <c r="D154" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A155" s="7"/>
+      <c r="A155" s="6"/>
       <c r="B155" s="4"/>
-      <c r="C155" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D155" s="5" t="s">
+      <c r="C155" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D155" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A156" s="7"/>
+      <c r="A156" s="6"/>
       <c r="B156" s="4"/>
       <c r="C156" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D156" s="5" t="s">
+      <c r="D156" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A157" s="7"/>
+      <c r="A157" s="6"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4" t="s">
         <v>224</v>
@@ -4330,8 +4324,8 @@
       </c>
     </row>
     <row r="158" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A158" s="8"/>
-      <c r="B158" s="5"/>
+      <c r="A158" s="6"/>
+      <c r="B158" s="4"/>
       <c r="C158" s="4" t="s">
         <v>144</v>
       </c>
@@ -4340,7 +4334,7 @@
       </c>
     </row>
     <row r="159" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A159" s="7" t="s">
+      <c r="A159" s="6" t="s">
         <v>226</v>
       </c>
       <c r="B159" s="4" t="str">
@@ -4350,32 +4344,32 @@
       <c r="C159" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D159" s="5" t="s">
+      <c r="D159" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A160" s="7"/>
+      <c r="A160" s="6"/>
       <c r="B160" s="4"/>
-      <c r="C160" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D160" s="5" t="s">
+      <c r="C160" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D160" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A161" s="7"/>
+      <c r="A161" s="6"/>
       <c r="B161" s="4"/>
       <c r="C161" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D161" s="5" t="s">
+      <c r="D161" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="162" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A162" s="7"/>
+      <c r="A162" s="6"/>
       <c r="B162" s="4"/>
       <c r="C162" s="4" t="s">
         <v>227</v>
@@ -4385,8 +4379,8 @@
       </c>
     </row>
     <row r="163" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A163" s="8"/>
-      <c r="B163" s="5"/>
+      <c r="A163" s="6"/>
+      <c r="B163" s="4"/>
       <c r="C163" s="4" t="s">
         <v>144</v>
       </c>
@@ -4395,7 +4389,7 @@
       </c>
     </row>
     <row r="164" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A164" s="7" t="s">
+      <c r="A164" s="6" t="s">
         <v>228</v>
       </c>
       <c r="B164" s="4" t="str">
@@ -4405,32 +4399,32 @@
       <c r="C164" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D164" s="5" t="s">
+      <c r="D164" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A165" s="7"/>
+      <c r="A165" s="6"/>
       <c r="B165" s="4"/>
-      <c r="C165" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D165" s="5" t="s">
+      <c r="C165" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D165" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A166" s="7"/>
+      <c r="A166" s="6"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D166" s="5" t="s">
+      <c r="D166" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A167" s="7"/>
+      <c r="A167" s="6"/>
       <c r="B167" s="4"/>
       <c r="C167" s="4" t="s">
         <v>229</v>
@@ -4440,7 +4434,7 @@
       </c>
     </row>
     <row r="168" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A168" s="7" t="s">
+      <c r="A168" s="6" t="s">
         <v>231</v>
       </c>
       <c r="B168" s="4" t="str">
@@ -4450,33 +4444,33 @@
       <c r="C168" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D168" s="5" t="s">
+      <c r="D168" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A169" s="7"/>
+      <c r="A169" s="6"/>
       <c r="B169" s="4"/>
-      <c r="C169" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D169" s="5" t="s">
+      <c r="C169" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D169" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A170" s="7"/>
+      <c r="A170" s="6"/>
       <c r="B170" s="4"/>
       <c r="C170" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D170" s="5" t="s">
+      <c r="D170" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A171" s="8"/>
-      <c r="B171" s="5"/>
+      <c r="A171" s="6"/>
+      <c r="B171" s="4"/>
       <c r="C171" s="4" t="s">
         <v>232</v>
       </c>
@@ -4485,7 +4479,7 @@
       </c>
     </row>
     <row r="172" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A172" s="7" t="s">
+      <c r="A172" s="6" t="s">
         <v>234</v>
       </c>
       <c r="B172" s="4" t="str">
@@ -4495,33 +4489,33 @@
       <c r="C172" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D172" s="5" t="s">
+      <c r="D172" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A173" s="7"/>
+      <c r="A173" s="6"/>
       <c r="B173" s="4"/>
-      <c r="C173" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D173" s="5" t="s">
+      <c r="C173" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D173" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A174" s="7"/>
+      <c r="A174" s="6"/>
       <c r="B174" s="4"/>
       <c r="C174" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D174" s="5" t="s">
+      <c r="D174" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A175" s="8"/>
-      <c r="B175" s="5"/>
+      <c r="A175" s="6"/>
+      <c r="B175" s="4"/>
       <c r="C175" s="4" t="s">
         <v>235</v>
       </c>
@@ -4530,7 +4524,7 @@
       </c>
     </row>
     <row r="176" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A176" s="7" t="s">
+      <c r="A176" s="6" t="s">
         <v>237</v>
       </c>
       <c r="B176" s="4" t="str">
@@ -4540,33 +4534,33 @@
       <c r="C176" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D176" s="5" t="s">
+      <c r="D176" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A177" s="7"/>
+      <c r="A177" s="6"/>
       <c r="B177" s="4"/>
-      <c r="C177" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D177" s="5" t="s">
+      <c r="C177" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D177" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A178" s="7"/>
+      <c r="A178" s="6"/>
       <c r="B178" s="4"/>
       <c r="C178" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D178" s="5" t="s">
+      <c r="D178" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A179" s="8"/>
-      <c r="B179" s="5"/>
+      <c r="A179" s="6"/>
+      <c r="B179" s="4"/>
       <c r="C179" s="4" t="s">
         <v>238</v>
       </c>
@@ -4575,7 +4569,7 @@
       </c>
     </row>
     <row r="180" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A180" s="7" t="s">
+      <c r="A180" s="6" t="s">
         <v>240</v>
       </c>
       <c r="B180" s="4" t="str">
@@ -4585,33 +4579,33 @@
       <c r="C180" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D180" s="5" t="s">
+      <c r="D180" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A181" s="7"/>
+      <c r="A181" s="6"/>
       <c r="B181" s="4"/>
-      <c r="C181" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D181" s="5" t="s">
+      <c r="C181" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D181" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A182" s="7"/>
+      <c r="A182" s="6"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D182" s="5" t="s">
+      <c r="D182" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A183" s="8"/>
-      <c r="B183" s="5"/>
+      <c r="A183" s="6"/>
+      <c r="B183" s="4"/>
       <c r="C183" s="4" t="s">
         <v>241</v>
       </c>
@@ -4620,7 +4614,7 @@
       </c>
     </row>
     <row r="184" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A184" s="7" t="s">
+      <c r="A184" s="6" t="s">
         <v>242</v>
       </c>
       <c r="B184" s="4" t="str">
@@ -4630,33 +4624,33 @@
       <c r="C184" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D184" s="5" t="s">
+      <c r="D184" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A185" s="7"/>
+      <c r="A185" s="6"/>
       <c r="B185" s="4"/>
-      <c r="C185" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D185" s="5" t="s">
+      <c r="C185" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D185" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A186" s="7"/>
+      <c r="A186" s="6"/>
       <c r="B186" s="4"/>
       <c r="C186" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D186" s="5" t="s">
+      <c r="D186" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A187" s="8"/>
-      <c r="B187" s="5"/>
+      <c r="A187" s="6"/>
+      <c r="B187" s="4"/>
       <c r="C187" s="4" t="s">
         <v>243</v>
       </c>
@@ -4665,7 +4659,7 @@
       </c>
     </row>
     <row r="188" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A188" s="7" t="s">
+      <c r="A188" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B188" s="4" t="str">
@@ -4675,33 +4669,33 @@
       <c r="C188" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D188" s="5" t="s">
+      <c r="D188" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A189" s="7"/>
+      <c r="A189" s="6"/>
       <c r="B189" s="4"/>
-      <c r="C189" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D189" s="5" t="s">
+      <c r="C189" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D189" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A190" s="7"/>
+      <c r="A190" s="6"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D190" s="5" t="s">
+      <c r="D190" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A191" s="8"/>
-      <c r="B191" s="5"/>
+      <c r="A191" s="6"/>
+      <c r="B191" s="4"/>
       <c r="C191" s="4" t="s">
         <v>246</v>
       </c>
@@ -4710,7 +4704,7 @@
       </c>
     </row>
     <row r="192" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A192" s="7" t="s">
+      <c r="A192" s="6" t="s">
         <v>248</v>
       </c>
       <c r="B192" s="4" t="str">
@@ -4720,32 +4714,32 @@
       <c r="C192" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D192" s="5" t="s">
+      <c r="D192" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A193" s="7"/>
+      <c r="A193" s="6"/>
       <c r="B193" s="4"/>
-      <c r="C193" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D193" s="5" t="s">
+      <c r="C193" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D193" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A194" s="7"/>
+      <c r="A194" s="6"/>
       <c r="B194" s="4"/>
       <c r="C194" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D194" s="5" t="s">
+      <c r="D194" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A195" s="7"/>
+      <c r="A195" s="6"/>
       <c r="B195" s="4"/>
       <c r="C195" s="4" t="s">
         <v>249</v>
@@ -4755,7 +4749,7 @@
       </c>
     </row>
     <row r="196" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A196" s="7"/>
+      <c r="A196" s="6"/>
       <c r="B196" s="4"/>
       <c r="C196" s="4" t="s">
         <v>251</v>
@@ -4765,7 +4759,7 @@
       </c>
     </row>
     <row r="197" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A197" s="7" t="s">
+      <c r="A197" s="6" t="s">
         <v>253</v>
       </c>
       <c r="B197" s="4" t="str">
@@ -4775,32 +4769,32 @@
       <c r="C197" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D197" s="5" t="s">
+      <c r="D197" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A198" s="7"/>
+      <c r="A198" s="6"/>
       <c r="B198" s="4"/>
-      <c r="C198" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D198" s="5" t="s">
+      <c r="C198" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D198" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A199" s="7"/>
+      <c r="A199" s="6"/>
       <c r="B199" s="4"/>
       <c r="C199" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D199" s="5" t="s">
+      <c r="D199" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A200" s="7"/>
+      <c r="A200" s="6"/>
       <c r="B200" s="4"/>
       <c r="C200" s="4" t="s">
         <v>254</v>
@@ -4810,7 +4804,7 @@
       </c>
     </row>
     <row r="201" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A201" s="8"/>
+      <c r="A201" s="6"/>
       <c r="B201" s="4"/>
       <c r="C201" s="4" t="s">
         <v>251</v>
@@ -4820,7 +4814,7 @@
       </c>
     </row>
     <row r="202" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A202" s="7" t="s">
+      <c r="A202" s="6" t="s">
         <v>257</v>
       </c>
       <c r="B202" s="4" t="str">
@@ -4830,32 +4824,32 @@
       <c r="C202" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D202" s="5" t="s">
+      <c r="D202" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="203" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A203" s="7"/>
+      <c r="A203" s="6"/>
       <c r="B203" s="4"/>
-      <c r="C203" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D203" s="5" t="s">
+      <c r="C203" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D203" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="204" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A204" s="7"/>
+      <c r="A204" s="6"/>
       <c r="B204" s="4"/>
       <c r="C204" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D204" s="5" t="s">
+      <c r="D204" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="205" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A205" s="7"/>
+      <c r="A205" s="6"/>
       <c r="B205" s="4"/>
       <c r="C205" s="4" t="s">
         <v>254</v>
@@ -4865,8 +4859,8 @@
       </c>
     </row>
     <row r="206" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A206" s="8"/>
-      <c r="B206" s="5"/>
+      <c r="A206" s="6"/>
+      <c r="B206" s="4"/>
       <c r="C206" s="4" t="s">
         <v>258</v>
       </c>
@@ -4875,7 +4869,7 @@
       </c>
     </row>
     <row r="207" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A207" s="7" t="s">
+      <c r="A207" s="6" t="s">
         <v>260</v>
       </c>
       <c r="B207" s="4" t="str">
@@ -4885,32 +4879,32 @@
       <c r="C207" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D207" s="5" t="s">
+      <c r="D207" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A208" s="7"/>
+      <c r="A208" s="6"/>
       <c r="B208" s="4"/>
-      <c r="C208" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D208" s="5" t="s">
+      <c r="C208" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D208" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="209" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A209" s="7"/>
+      <c r="A209" s="6"/>
       <c r="B209" s="4"/>
       <c r="C209" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D209" s="5" t="s">
+      <c r="D209" s="4" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="210" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A210" s="7" t="s">
+      <c r="A210" s="6" t="s">
         <v>263</v>
       </c>
       <c r="B210" s="4" t="str">
@@ -4920,32 +4914,32 @@
       <c r="C210" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D210" s="5" t="s">
+      <c r="D210" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="211" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A211" s="7"/>
+      <c r="A211" s="6"/>
       <c r="B211" s="4"/>
-      <c r="C211" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D211" s="5" t="s">
+      <c r="C211" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D211" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="212" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A212" s="7"/>
+      <c r="A212" s="6"/>
       <c r="B212" s="4"/>
       <c r="C212" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D212" s="5" t="s">
+      <c r="D212" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="213" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A213" s="7"/>
+      <c r="A213" s="6"/>
       <c r="B213" s="4"/>
       <c r="C213" s="4" t="s">
         <v>265</v>
@@ -4955,17 +4949,17 @@
       </c>
     </row>
     <row r="214" s="1" customFormat="1" ht="42" spans="1:4">
-      <c r="A214" s="8"/>
-      <c r="B214" s="5"/>
+      <c r="A214" s="6"/>
+      <c r="B214" s="4"/>
       <c r="C214" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="D214" s="9" t="s">
+      <c r="D214" s="7" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="215" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A215" s="7" t="s">
+      <c r="A215" s="6" t="s">
         <v>269</v>
       </c>
       <c r="B215" s="4" t="str">
@@ -4975,32 +4969,32 @@
       <c r="C215" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D215" s="5" t="s">
+      <c r="D215" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="216" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A216" s="7"/>
+      <c r="A216" s="6"/>
       <c r="B216" s="4"/>
-      <c r="C216" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D216" s="5" t="s">
+      <c r="C216" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D216" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="217" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A217" s="7"/>
+      <c r="A217" s="6"/>
       <c r="B217" s="4"/>
       <c r="C217" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D217" s="5" t="s">
+      <c r="D217" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="218" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A218" s="7"/>
+      <c r="A218" s="6"/>
       <c r="B218" s="4"/>
       <c r="C218" s="4" t="s">
         <v>265</v>
@@ -5010,17 +5004,17 @@
       </c>
     </row>
     <row r="219" s="1" customFormat="1" ht="42" spans="1:4">
-      <c r="A219" s="8"/>
-      <c r="B219" s="5"/>
+      <c r="A219" s="6"/>
+      <c r="B219" s="4"/>
       <c r="C219" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D219" s="9" t="s">
+      <c r="D219" s="7" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="220" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A220" s="7" t="s">
+      <c r="A220" s="6" t="s">
         <v>272</v>
       </c>
       <c r="B220" s="4" t="str">
@@ -5030,32 +5024,32 @@
       <c r="C220" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D220" s="5" t="s">
+      <c r="D220" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="221" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A221" s="7"/>
+      <c r="A221" s="6"/>
       <c r="B221" s="4"/>
-      <c r="C221" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D221" s="5" t="s">
+      <c r="C221" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D221" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="222" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A222" s="7"/>
+      <c r="A222" s="6"/>
       <c r="B222" s="4"/>
       <c r="C222" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D222" s="5" t="s">
+      <c r="D222" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="223" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A223" s="7"/>
+      <c r="A223" s="6"/>
       <c r="B223" s="4"/>
       <c r="C223" s="4" t="s">
         <v>265</v>
@@ -5065,17 +5059,17 @@
       </c>
     </row>
     <row r="224" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A224" s="8"/>
-      <c r="B224" s="5"/>
+      <c r="A224" s="6"/>
+      <c r="B224" s="4"/>
       <c r="C224" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="D224" s="9" t="s">
+      <c r="D224" s="7" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="225" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A225" s="7" t="s">
+      <c r="A225" s="6" t="s">
         <v>275</v>
       </c>
       <c r="B225" s="4" t="str">
@@ -5085,32 +5079,32 @@
       <c r="C225" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D225" s="5" t="s">
+      <c r="D225" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="226" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A226" s="7"/>
+      <c r="A226" s="6"/>
       <c r="B226" s="4"/>
-      <c r="C226" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D226" s="5" t="s">
+      <c r="C226" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D226" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="227" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A227" s="7"/>
+      <c r="A227" s="6"/>
       <c r="B227" s="4"/>
       <c r="C227" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D227" s="5" t="s">
+      <c r="D227" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="228" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A228" s="7"/>
+      <c r="A228" s="6"/>
       <c r="B228" s="4"/>
       <c r="C228" s="4" t="s">
         <v>265</v>
@@ -5120,17 +5114,17 @@
       </c>
     </row>
     <row r="229" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A229" s="8"/>
-      <c r="B229" s="5"/>
+      <c r="A229" s="6"/>
+      <c r="B229" s="4"/>
       <c r="C229" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="D229" s="9" t="s">
+      <c r="D229" s="7" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="230" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A230" s="7" t="s">
+      <c r="A230" s="6" t="s">
         <v>278</v>
       </c>
       <c r="B230" s="4" t="str">
@@ -5140,32 +5134,32 @@
       <c r="C230" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D230" s="5" t="s">
+      <c r="D230" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="231" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A231" s="7"/>
+      <c r="A231" s="6"/>
       <c r="B231" s="4"/>
-      <c r="C231" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D231" s="5" t="s">
+      <c r="C231" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D231" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="232" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A232" s="7"/>
+      <c r="A232" s="6"/>
       <c r="B232" s="4"/>
       <c r="C232" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D232" s="5" t="s">
+      <c r="D232" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="233" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A233" s="7"/>
+      <c r="A233" s="6"/>
       <c r="B233" s="4"/>
       <c r="C233" s="4" t="s">
         <v>265</v>
@@ -5174,28 +5168,28 @@
         <v>266</v>
       </c>
     </row>
-    <row r="234" s="1" customFormat="1" ht="42" spans="1:4">
-      <c r="A234" s="7"/>
+    <row r="234" s="1" customFormat="1" ht="21" spans="1:4">
+      <c r="A234" s="6"/>
       <c r="B234" s="4"/>
       <c r="C234" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="D234" s="9" t="s">
+      <c r="D234" s="7" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="235" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A235" s="7"/>
+      <c r="A235" s="6"/>
       <c r="B235" s="4"/>
       <c r="C235" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D235" s="9" t="s">
+      <c r="D235" s="7" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="236" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A236" s="7" t="s">
+      <c r="A236" s="6" t="s">
         <v>283</v>
       </c>
       <c r="B236" s="4" t="str">
@@ -5205,32 +5199,32 @@
       <c r="C236" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D236" s="5" t="s">
+      <c r="D236" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="237" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A237" s="7"/>
+      <c r="A237" s="6"/>
       <c r="B237" s="4"/>
-      <c r="C237" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D237" s="5" t="s">
+      <c r="C237" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D237" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="238" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A238" s="7"/>
+      <c r="A238" s="6"/>
       <c r="B238" s="4"/>
       <c r="C238" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D238" s="5" t="s">
+      <c r="D238" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="239" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A239" s="7"/>
+      <c r="A239" s="6"/>
       <c r="B239" s="4"/>
       <c r="C239" s="4" t="s">
         <v>265</v>
@@ -5239,28 +5233,28 @@
         <v>266</v>
       </c>
     </row>
-    <row r="240" s="1" customFormat="1" ht="42" spans="1:4">
-      <c r="A240" s="7"/>
+    <row r="240" s="1" customFormat="1" ht="21" spans="1:4">
+      <c r="A240" s="6"/>
       <c r="B240" s="4"/>
       <c r="C240" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="D240" s="9" t="s">
+      <c r="D240" s="7" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="241" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A241" s="8"/>
-      <c r="B241" s="5"/>
+      <c r="A241" s="6"/>
+      <c r="B241" s="4"/>
       <c r="C241" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D241" s="9" t="s">
+      <c r="D241" s="7" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="242" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A242" s="7" t="s">
+      <c r="A242" s="6" t="s">
         <v>286</v>
       </c>
       <c r="B242" s="4" t="str">
@@ -5270,43 +5264,43 @@
       <c r="C242" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D242" s="5" t="s">
+      <c r="D242" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="243" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A243" s="7"/>
+      <c r="A243" s="6"/>
       <c r="B243" s="4"/>
-      <c r="C243" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D243" s="5" t="s">
+      <c r="C243" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D243" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="244" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A244" s="7"/>
+      <c r="A244" s="6"/>
       <c r="B244" s="4"/>
       <c r="C244" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D244" s="5" t="s">
+      <c r="D244" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="245" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A245" s="7"/>
+      <c r="A245" s="6"/>
       <c r="B245" s="4"/>
       <c r="C245" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="D245" s="5" t="s">
+      <c r="D245" s="4" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="246" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A246" s="8"/>
-      <c r="B246" s="5"/>
+      <c r="A246" s="6"/>
+      <c r="B246" s="4"/>
       <c r="C246" s="4" t="s">
         <v>289</v>
       </c>
@@ -5315,7 +5309,7 @@
       </c>
     </row>
     <row r="247" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A247" s="7" t="s">
+      <c r="A247" s="6" t="s">
         <v>291</v>
       </c>
       <c r="B247" s="4" t="str">
@@ -5325,53 +5319,53 @@
       <c r="C247" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D247" s="5" t="s">
+      <c r="D247" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="248" s="1" customFormat="1" ht="63" spans="1:4">
-      <c r="A248" s="7"/>
+      <c r="A248" s="6"/>
       <c r="B248" s="4"/>
-      <c r="C248" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D248" s="5" t="s">
+      <c r="C248" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D248" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="249" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A249" s="7"/>
+      <c r="A249" s="6"/>
       <c r="B249" s="4"/>
       <c r="C249" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D249" s="5" t="s">
+      <c r="D249" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="250" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A250" s="7"/>
+      <c r="A250" s="6"/>
       <c r="B250" s="4"/>
       <c r="C250" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="D250" s="5" t="s">
-        <v>288</v>
+        <v>292</v>
+      </c>
+      <c r="D250" s="4" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="251" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A251" s="8"/>
-      <c r="B251" s="5"/>
+      <c r="A251" s="6"/>
+      <c r="B251" s="4"/>
       <c r="C251" s="4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="252" s="1" customFormat="1" ht="21" spans="1:4">
       <c r="A252" s="4" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B252" s="4" t="str">
         <f>'Mars Test Condition'!D59</f>
@@ -5380,17 +5374,17 @@
       <c r="C252" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D252" s="5" t="s">
+      <c r="D252" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="253" s="1" customFormat="1" ht="63" spans="1:4">
       <c r="A253" s="4"/>
       <c r="B253" s="4"/>
-      <c r="C253" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D253" s="5" t="s">
+      <c r="C253" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D253" s="4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -5400,18 +5394,18 @@
       <c r="C254" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D254" s="5" t="s">
+      <c r="D254" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="255" s="1" customFormat="1" ht="21" spans="1:4">
-      <c r="A255" s="5"/>
-      <c r="B255" s="5"/>
+      <c r="A255" s="4"/>
+      <c r="B255" s="4"/>
       <c r="C255" s="4" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="256" s="1" customFormat="1" ht="21" spans="3:3">
@@ -5472,7 +5466,7 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" s="1" customFormat="1" ht="21" spans="3:3">
-      <c r="C275" s="10"/>
+      <c r="C275" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="116">

</xml_diff>

<commit_message>
Update TestCases & PageFactory
</commit_message>
<xml_diff>
--- a/Mars_Ava.xlsx
+++ b/Mars_Ava.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9264" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9264"/>
   </bookViews>
   <sheets>
     <sheet name="Mars Test Condition" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306">
   <si>
     <t xml:space="preserve">Test Condition ID </t>
   </si>
@@ -35,7 +35,7 @@
     <t>Share Skill</t>
   </si>
   <si>
-    <t>Validate "Share Skill" button</t>
+    <t>Validate "Share Skill" button on Home page</t>
   </si>
   <si>
     <t>Check if seller is navigated to the detailed form page</t>
@@ -221,6 +221,15 @@
     <t>TC_014</t>
   </si>
   <si>
+    <t>Validate "Cancel" button on "Share Skill" page</t>
+  </si>
+  <si>
+    <t>Check if seller is able to cancel skill details</t>
+  </si>
+  <si>
+    <t>TC_015</t>
+  </si>
+  <si>
     <t>Validate "Save" button on "Share Skill" page</t>
   </si>
   <si>
@@ -230,31 +239,24 @@
     <t>Check if seller is able to save skill details with valid information</t>
   </si>
   <si>
-    <t>TC_015</t>
-  </si>
-  <si>
-    <t>Validate "Cancel" button on "Share Skill" page</t>
-  </si>
-  <si>
-    <t>Check if seller is able to cancel skill details</t>
-  </si>
-  <si>
     <t>TC_016</t>
   </si>
   <si>
     <t>Manage Listings</t>
   </si>
   <si>
-    <t>Validate "Manage Listings" page when there is no service listings</t>
-  </si>
-  <si>
-    <t>Check if seller is able to see no listing message "You do not have any service listings!"</t>
+    <t>Validate "Manage Listings" page 
+when there is no service listings</t>
+  </si>
+  <si>
+    <t>Check if seller is able to see message "You do not have any service listings!"</t>
   </si>
   <si>
     <t>TC_017</t>
   </si>
   <si>
-    <t>Validate "Active" status on "Manage Listings" page</t>
+    <t>Validate "Active" status on "Manage Listings" page 
+when there are service listings</t>
   </si>
   <si>
     <t>Check if seller is able to change activated status to deactivated</t>
@@ -266,7 +268,7 @@
     <t>TC_018</t>
   </si>
   <si>
-    <t>Validate the eye icon of "Actions" on "Manage Listings" page</t>
+    <t>Validate the eye icon of "Actions" on "Manage Listings" page when there are service listings</t>
   </si>
   <si>
     <t>Check if seller is able to view the details of the selected service</t>
@@ -275,7 +277,7 @@
     <t>TC_019</t>
   </si>
   <si>
-    <t>Validate the write icon of "Actions" on "Manage Listings" page</t>
+    <t>Validate the write icon of "Actions" on "Manage Listings" page when there are service listings</t>
   </si>
   <si>
     <t>Check if seller is able to edit the selected service</t>
@@ -284,7 +286,7 @@
     <t>TC_020</t>
   </si>
   <si>
-    <t>Validate the remove icon of "Actions" on "Manage Listings" page</t>
+    <t>Validate the remove icon of "Actions" on "Manage Listings" page when there are service listings</t>
   </si>
   <si>
     <t>Check if seller is able to delete the selected service</t>
@@ -296,7 +298,8 @@
     <t>TC_021</t>
   </si>
   <si>
-    <t>Validate the icon of the next page on "Manage Listings" page</t>
+    <t>Validate the icon of the next page on "Manage Listings" page 
+when there are more than 2 pages service listings</t>
   </si>
   <si>
     <t>Check if seller is able to navigate to the next page</t>
@@ -305,7 +308,8 @@
     <t>TC_022</t>
   </si>
   <si>
-    <t>Validate the icon of the previous page on "Manage Listings" page</t>
+    <t>Validate the icon of the previous page on "Manage Listings" page 
+when there are more than 2 pages service listings</t>
   </si>
   <si>
     <t>Check if seller is able to navigate to the previous page</t>
@@ -314,7 +318,8 @@
     <t>TC_023</t>
   </si>
   <si>
-    <t>Validate the number of page on "Manage Listings" page</t>
+    <t>Validate the number of page on "Manage Listings" page 
+when there are more than 2 pages service listings</t>
   </si>
   <si>
     <t>Check if seller is able to navigate to the selected page</t>
@@ -358,7 +363,7 @@
     <t>Seller should be able to login to the home page</t>
   </si>
   <si>
-    <t>Step 3: Click on the the "Share Skill" button</t>
+    <t>Step 3: Click on the "Share Skill" button on Home page</t>
   </si>
   <si>
     <t>Seller should be able to navigate to the detailed form page</t>
@@ -777,54 +782,64 @@
     <t>TC_014_01</t>
   </si>
   <si>
-    <t>Step 4: Input every field with any invalid information</t>
-  </si>
-  <si>
-    <t>Seller should be able to see the red error message under field</t>
+    <t>Step 4: Input every field with all valid information</t>
+  </si>
+  <si>
+    <t>Seller should be able to see no red error message</t>
+  </si>
+  <si>
+    <t>Complex</t>
+  </si>
+  <si>
+    <t>Step 5: Click on the "Cancel" button at the end of the "Share Skill" page</t>
+  </si>
+  <si>
+    <t>Seller should be able to back to the previous page</t>
+  </si>
+  <si>
+    <t>TC_015_01</t>
+  </si>
+  <si>
+    <t>Step 4: Input every field with all invalid information</t>
+  </si>
+  <si>
+    <t>Seller should be able to see the red error messages under fields</t>
   </si>
   <si>
     <t>Step 5: Click on the "Save" button at the end of the "Share Skill" page</t>
   </si>
   <si>
-    <t>Seller should be able to see the red error message "Please complete the form correctly."</t>
-  </si>
-  <si>
-    <t>TC_014_02</t>
-  </si>
-  <si>
-    <t>Step 4: Input every field with all valid information</t>
-  </si>
-  <si>
-    <t>Seller should be able to see no red error message</t>
-  </si>
-  <si>
-    <t>Complex</t>
-  </si>
-  <si>
-    <t>Seller should be able to see the popup message "Service Listing Added successfully."</t>
-  </si>
-  <si>
-    <t>TC_015_01</t>
-  </si>
-  <si>
-    <t>Step 5: Click on the "Cancel" button at the end of the "Share Skill" page</t>
-  </si>
-  <si>
-    <t>Seller should be able to back to the previous page</t>
+    <t>Seller should be able to see the popup message "Please complete the form correctly." on "Share Skill" page</t>
+  </si>
+  <si>
+    <t>TC_015_02</t>
+  </si>
+  <si>
+    <t>Step 4: Input every field with any valid information</t>
+  </si>
+  <si>
+    <t>Seller should be able to see no any red error messages</t>
+  </si>
+  <si>
+    <t>Seller should be able to see the popup message "Service Listing Added successfully." and 
+navigate to "Manage Listings" page with saved skill.</t>
   </si>
   <si>
     <t>TC_016_01</t>
   </si>
   <si>
-    <t>Step 3: Click on the the "Manage Listings" tab</t>
-  </si>
-  <si>
-    <t>Seller should be able to see no listing message "You do not have any service listings!"</t>
+    <t>Step 3: Click on the "Manage Listings" tab when there is no service listings</t>
+  </si>
+  <si>
+    <t>Seller should be able to see message "You do not have any service listings!" with no listing.</t>
   </si>
   <si>
     <t>TC_017_01</t>
   </si>
   <si>
+    <t>Step 3: Click on the "Manage Listings" tab when there are service listings</t>
+  </si>
+  <si>
     <t>Seller should be able to navigate to liststings with service page</t>
   </si>
   <si>
@@ -892,6 +907,9 @@
   </si>
   <si>
     <t>TC_021_01</t>
+  </si>
+  <si>
+    <t>Step 3: Click on the "Manage Listings" tab when there are more than 2 pages service listings</t>
   </si>
   <si>
     <t>Step 4: Select the first page</t>
@@ -935,10 +953,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -969,6 +987,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -976,29 +1010,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1012,39 +1041,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1058,40 +1086,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1105,9 +1102,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1128,25 +1146,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1158,61 +1176,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1224,55 +1194,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1290,7 +1212,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1302,13 +1320,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1319,6 +1337,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1337,10 +1379,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1364,65 +1432,15 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1440,134 +1458,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1592,16 +1610,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1882,8 +1894,8 @@
   <sheetPr/>
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" outlineLevelCol="6"/>
@@ -1904,7 +1916,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1912,7 +1924,7 @@
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1926,7 +1938,7 @@
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1936,7 +1948,7 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:4">
       <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
         <v>11</v>
@@ -1944,7 +1956,7 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:4">
       <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
         <v>12</v>
@@ -1952,12 +1964,12 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:7">
       <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
@@ -1965,7 +1977,7 @@
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1975,7 +1987,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:4">
       <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
         <v>17</v>
@@ -1983,7 +1995,7 @@
     </row>
     <row r="9" s="1" customFormat="1" spans="1:4">
       <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
         <v>12</v>
@@ -1991,7 +2003,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:4">
       <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
         <v>13</v>
@@ -2001,7 +2013,7 @@
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
@@ -2011,7 +2023,7 @@
     </row>
     <row r="12" s="1" customFormat="1" spans="1:4">
       <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
         <v>21</v>
@@ -2021,7 +2033,7 @@
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
@@ -2031,7 +2043,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:4">
       <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
         <v>25</v>
@@ -2039,7 +2051,7 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:4">
       <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
         <v>26</v>
@@ -2047,7 +2059,7 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:4">
       <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
         <v>12</v>
@@ -2055,7 +2067,7 @@
     </row>
     <row r="17" s="1" customFormat="1" spans="1:4">
       <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -2065,7 +2077,7 @@
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="4" t="s">
         <v>28</v>
       </c>
@@ -2075,7 +2087,7 @@
     </row>
     <row r="19" s="1" customFormat="1" spans="1:4">
       <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
         <v>30</v>
@@ -2085,7 +2097,7 @@
       <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
@@ -2095,7 +2107,7 @@
     </row>
     <row r="21" s="1" customFormat="1" spans="1:4">
       <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
         <v>34</v>
@@ -2105,7 +2117,7 @@
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="4" t="s">
         <v>36</v>
       </c>
@@ -2115,7 +2127,7 @@
     </row>
     <row r="23" s="1" customFormat="1" spans="1:4">
       <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
         <v>38</v>
@@ -2123,7 +2135,7 @@
     </row>
     <row r="24" s="1" customFormat="1" spans="1:4">
       <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
         <v>39</v>
@@ -2131,7 +2143,7 @@
     </row>
     <row r="25" s="1" customFormat="1" spans="1:4">
       <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
         <v>40</v>
@@ -2139,7 +2151,7 @@
     </row>
     <row r="26" s="1" customFormat="1" spans="1:4">
       <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
         <v>41</v>
@@ -2147,7 +2159,7 @@
     </row>
     <row r="27" s="1" customFormat="1" spans="1:4">
       <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
         <v>42</v>
@@ -2155,7 +2167,7 @@
     </row>
     <row r="28" s="1" customFormat="1" spans="1:4">
       <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
         <v>43</v>
@@ -2163,7 +2175,7 @@
     </row>
     <row r="29" s="1" customFormat="1" spans="1:4">
       <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
         <v>44</v>
@@ -2171,7 +2183,7 @@
     </row>
     <row r="30" s="1" customFormat="1" spans="1:4">
       <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
         <v>45</v>
@@ -2179,7 +2191,7 @@
     </row>
     <row r="31" s="1" customFormat="1" spans="1:4">
       <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
         <v>46</v>
@@ -2187,7 +2199,7 @@
     </row>
     <row r="32" s="1" customFormat="1" spans="1:4">
       <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
         <v>47</v>
@@ -2197,7 +2209,7 @@
       <c r="A33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="4" t="s">
         <v>49</v>
       </c>
@@ -2207,7 +2219,7 @@
     </row>
     <row r="34" s="1" customFormat="1" spans="1:4">
       <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
         <v>51</v>
@@ -2217,7 +2229,7 @@
       <c r="A35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="4" t="s">
         <v>53</v>
       </c>
@@ -2227,7 +2239,7 @@
     </row>
     <row r="36" s="1" customFormat="1" spans="1:4">
       <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="B36" s="5"/>
       <c r="C36" s="4"/>
       <c r="D36" s="1" t="s">
         <v>25</v>
@@ -2235,7 +2247,7 @@
     </row>
     <row r="37" s="1" customFormat="1" spans="1:4">
       <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="4"/>
       <c r="D37" s="1" t="s">
         <v>26</v>
@@ -2243,7 +2255,7 @@
     </row>
     <row r="38" s="1" customFormat="1" spans="1:4">
       <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="4"/>
       <c r="D38" s="1" t="s">
         <v>12</v>
@@ -2251,7 +2263,7 @@
     </row>
     <row r="39" s="1" customFormat="1" spans="1:4">
       <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="4"/>
       <c r="D39" s="1" t="s">
         <v>13</v>
@@ -2261,7 +2273,7 @@
       <c r="A40" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="5"/>
       <c r="C40" s="4" t="s">
         <v>55</v>
       </c>
@@ -2271,7 +2283,7 @@
     </row>
     <row r="41" s="1" customFormat="1" spans="1:4">
       <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="B41" s="5"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
         <v>57</v>
@@ -2281,7 +2293,7 @@
       <c r="A42" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="5"/>
       <c r="C42" s="4" t="s">
         <v>59</v>
       </c>
@@ -2291,7 +2303,7 @@
     </row>
     <row r="43" s="1" customFormat="1" spans="1:4">
       <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="B43" s="5"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
         <v>61</v>
@@ -2299,7 +2311,7 @@
     </row>
     <row r="44" s="1" customFormat="1" spans="1:4">
       <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="4"/>
       <c r="D44" s="1" t="s">
         <v>62</v>
@@ -2309,7 +2321,7 @@
       <c r="A45" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="4"/>
+      <c r="B45" s="5"/>
       <c r="C45" s="4" t="s">
         <v>64</v>
       </c>
@@ -2319,7 +2331,7 @@
     </row>
     <row r="46" s="1" customFormat="1" spans="1:4">
       <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+      <c r="B46" s="5"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4" t="s">
         <v>66</v>
@@ -2329,8 +2341,8 @@
       <c r="A47" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4" t="s">
+      <c r="B47" s="5"/>
+      <c r="C47" s="11" t="s">
         <v>68</v>
       </c>
       <c r="D47" s="4" t="s">
@@ -2338,33 +2350,33 @@
       </c>
     </row>
     <row r="48" s="1" customFormat="1" spans="1:4">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
+      <c r="A48" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="D48" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" s="1" customFormat="1" spans="1:4">
-      <c r="A49" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="13" t="s">
-        <v>72</v>
-      </c>
+      <c r="A49" s="4"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" s="1" customFormat="1" spans="1:4">
-      <c r="A50" s="13" t="s">
+    <row r="50" s="1" customFormat="1" ht="42" spans="1:4">
+      <c r="A50" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="12" t="s">
         <v>76</v>
       </c>
       <c r="D50" s="4" t="s">
@@ -2375,7 +2387,7 @@
       <c r="A51" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B51" s="4"/>
+      <c r="B51" s="5"/>
       <c r="C51" s="6" t="s">
         <v>79</v>
       </c>
@@ -2385,30 +2397,30 @@
     </row>
     <row r="52" s="1" customFormat="1" spans="1:4">
       <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
+      <c r="B52" s="5"/>
       <c r="C52" s="6"/>
       <c r="D52" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="53" s="1" customFormat="1" spans="1:4">
-      <c r="A53" s="13" t="s">
+    <row r="53" s="1" customFormat="1" ht="42" spans="1:4">
+      <c r="A53" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="14" t="s">
+      <c r="B53" s="5"/>
+      <c r="C53" s="12" t="s">
         <v>83</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" s="1" customFormat="1" spans="1:4">
-      <c r="A54" s="13" t="s">
+    <row r="54" s="1" customFormat="1" ht="42" spans="1:4">
+      <c r="A54" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="14" t="s">
+      <c r="B54" s="5"/>
+      <c r="C54" s="12" t="s">
         <v>86</v>
       </c>
       <c r="D54" s="4" t="s">
@@ -2419,7 +2431,7 @@
       <c r="A55" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B55" s="4"/>
+      <c r="B55" s="5"/>
       <c r="C55" s="6" t="s">
         <v>89</v>
       </c>
@@ -2429,42 +2441,42 @@
     </row>
     <row r="56" s="1" customFormat="1" spans="1:4">
       <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
+      <c r="B56" s="5"/>
       <c r="C56" s="6"/>
       <c r="D56" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="57" s="1" customFormat="1" spans="1:4">
+    <row r="57" s="1" customFormat="1" ht="42" spans="1:4">
       <c r="A57" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4" t="s">
+      <c r="B57" s="5"/>
+      <c r="C57" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="58" s="1" customFormat="1" spans="1:4">
+    <row r="58" s="1" customFormat="1" ht="42" spans="1:4">
       <c r="A58" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4" t="s">
+      <c r="B58" s="5"/>
+      <c r="C58" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="59" s="1" customFormat="1" spans="1:4">
+    <row r="59" s="1" customFormat="1" ht="42" spans="1:4">
       <c r="A59" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4" t="s">
+      <c r="B59" s="5"/>
+      <c r="C59" s="6" t="s">
         <v>99</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -2524,7 +2536,7 @@
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A48:A49"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B2:B49"/>
@@ -2541,7 +2553,7 @@
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C42:C44"/>
     <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C48:C49"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="C55:C56"/>
   </mergeCells>
@@ -2556,16 +2568,16 @@
   <sheetPr/>
   <dimension ref="A1:G275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D94" workbookViewId="0">
-      <selection activeCell="D217" sqref="D217"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="C255" sqref="C255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="19.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="130" customWidth="1"/>
-    <col min="3" max="3" width="116.444444444444" style="2" customWidth="1"/>
-    <col min="4" max="4" width="156.777777777778" customWidth="1"/>
+    <col min="2" max="2" width="102.222222222222" customWidth="1"/>
+    <col min="3" max="3" width="122.962962962963" style="2" customWidth="1"/>
+    <col min="4" max="4" width="155.333333333333" customWidth="1"/>
     <col min="5" max="5" width="15.8518518518519" customWidth="1"/>
     <col min="6" max="6" width="16.5740740740741"/>
     <col min="7" max="7" width="13.5740740740741"/>
@@ -5111,7 +5123,7 @@
       <c r="C179" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="D179" s="9" t="s">
+      <c r="D179" s="8" t="s">
         <v>241</v>
       </c>
       <c r="F179" s="5" t="s">
@@ -5168,7 +5180,7 @@
       <c r="C183" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D183" s="9" t="s">
+      <c r="D183" s="8" t="s">
         <v>241</v>
       </c>
       <c r="F183" s="5" t="s">
@@ -5295,7 +5307,7 @@
       </c>
       <c r="B192" s="4" t="str">
         <f>'Mars Test Condition'!D47</f>
-        <v>Check if seller is able to save skill details with invalid information</v>
+        <v>Check if seller is able to cancel skill details</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>108</v>
@@ -5343,29 +5355,29 @@
         <v>252</v>
       </c>
       <c r="F195" s="5" t="s">
-        <v>118</v>
+        <v>253</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A196" s="7"/>
       <c r="B196" s="4"/>
       <c r="C196" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F196" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="D196" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F196" s="5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A197" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B197" s="4" t="str">
         <f>'Mars Test Condition'!D48</f>
-        <v>Check if seller is able to save skill details with valid information</v>
+        <v>Check if seller is able to save skill details with invalid information</v>
       </c>
       <c r="C197" s="4" t="s">
         <v>108</v>
@@ -5407,35 +5419,35 @@
       <c r="A200" s="7"/>
       <c r="B200" s="4"/>
       <c r="C200" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F200" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A201" s="7"/>
       <c r="B201" s="4"/>
       <c r="C201" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F201" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="D201" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F201" s="5" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="202" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A202" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B202" s="4" t="str">
         <f>'Mars Test Condition'!D49</f>
-        <v>Check if seller is able to cancel skill details</v>
+        <v>Check if seller is able to save skill details with valid information</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>108</v>
@@ -5477,35 +5489,35 @@
       <c r="A205" s="7"/>
       <c r="B205" s="4"/>
       <c r="C205" s="4" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="F205" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="206" s="1" customFormat="1" ht="21" spans="1:6">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="206" s="1" customFormat="1" ht="42" spans="1:6">
       <c r="A206" s="7"/>
       <c r="B206" s="4"/>
       <c r="C206" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D206" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
+      </c>
+      <c r="D206" s="8" t="s">
+        <v>264</v>
       </c>
       <c r="F206" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="207" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A207" s="7" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B207" s="4" t="str">
         <f>'Mars Test Condition'!D50</f>
-        <v>Check if seller is able to see no listing message "You do not have any service listings!"</v>
+        <v>Check if seller is able to see message "You do not have any service listings!"</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>108</v>
@@ -5534,10 +5546,10 @@
       <c r="A209" s="7"/>
       <c r="B209" s="4"/>
       <c r="C209" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D209" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F209" s="5" t="s">
         <v>110</v>
@@ -5545,7 +5557,7 @@
     </row>
     <row r="210" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A210" s="7" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B210" s="4" t="str">
         <f>'Mars Test Condition'!D51</f>
@@ -5578,10 +5590,10 @@
       <c r="A212" s="7"/>
       <c r="B212" s="4"/>
       <c r="C212" s="4" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D212" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F212" s="5" t="s">
         <v>110</v>
@@ -5591,23 +5603,23 @@
       <c r="A213" s="7"/>
       <c r="B213" s="4"/>
       <c r="C213" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F213" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="214" s="1" customFormat="1" ht="42" spans="1:6">
+    <row r="214" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A214" s="7"/>
       <c r="B214" s="4"/>
       <c r="C214" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D214" s="8" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="F214" s="5" t="s">
         <v>118</v>
@@ -5615,7 +5627,7 @@
     </row>
     <row r="215" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A215" s="7" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B215" s="4" t="str">
         <f>'Mars Test Condition'!D52</f>
@@ -5648,10 +5660,10 @@
       <c r="A217" s="7"/>
       <c r="B217" s="4"/>
       <c r="C217" s="4" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D217" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F217" s="5" t="s">
         <v>110</v>
@@ -5661,23 +5673,23 @@
       <c r="A218" s="7"/>
       <c r="B218" s="4"/>
       <c r="C218" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F218" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="219" s="1" customFormat="1" ht="42" spans="1:6">
+    <row r="219" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A219" s="7"/>
       <c r="B219" s="4"/>
       <c r="C219" s="4" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D219" s="8" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F219" s="5" t="s">
         <v>118</v>
@@ -5685,7 +5697,7 @@
     </row>
     <row r="220" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A220" s="7" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B220" s="4" t="str">
         <f>'Mars Test Condition'!D53</f>
@@ -5718,10 +5730,10 @@
       <c r="A222" s="7"/>
       <c r="B222" s="4"/>
       <c r="C222" s="4" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F222" s="5" t="s">
         <v>110</v>
@@ -5731,10 +5743,10 @@
       <c r="A223" s="7"/>
       <c r="B223" s="4"/>
       <c r="C223" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F223" s="5" t="s">
         <v>110</v>
@@ -5744,10 +5756,10 @@
       <c r="A224" s="7"/>
       <c r="B224" s="4"/>
       <c r="C224" s="4" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D224" s="8" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F224" s="5" t="s">
         <v>118</v>
@@ -5755,7 +5767,7 @@
     </row>
     <row r="225" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A225" s="7" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B225" s="4" t="str">
         <f>'Mars Test Condition'!D54</f>
@@ -5788,10 +5800,10 @@
       <c r="A227" s="7"/>
       <c r="B227" s="4"/>
       <c r="C227" s="4" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D227" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F227" s="5" t="s">
         <v>110</v>
@@ -5801,10 +5813,10 @@
       <c r="A228" s="7"/>
       <c r="B228" s="4"/>
       <c r="C228" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F228" s="5" t="s">
         <v>110</v>
@@ -5814,10 +5826,10 @@
       <c r="A229" s="7"/>
       <c r="B229" s="4"/>
       <c r="C229" s="4" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D229" s="8" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F229" s="5" t="s">
         <v>118</v>
@@ -5825,7 +5837,7 @@
     </row>
     <row r="230" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A230" s="7" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B230" s="4" t="str">
         <f>'Mars Test Condition'!D55</f>
@@ -5858,10 +5870,10 @@
       <c r="A232" s="7"/>
       <c r="B232" s="4"/>
       <c r="C232" s="4" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D232" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F232" s="5" t="s">
         <v>110</v>
@@ -5871,10 +5883,10 @@
       <c r="A233" s="7"/>
       <c r="B233" s="4"/>
       <c r="C233" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F233" s="5" t="s">
         <v>110</v>
@@ -5884,31 +5896,31 @@
       <c r="A234" s="7"/>
       <c r="B234" s="4"/>
       <c r="C234" s="4" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D234" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F234" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="235" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A235" s="7"/>
       <c r="B235" s="4"/>
       <c r="C235" s="1" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D235" s="8" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="F235" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="236" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A236" s="7" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B236" s="4" t="str">
         <f>'Mars Test Condition'!D56</f>
@@ -5941,10 +5953,10 @@
       <c r="A238" s="7"/>
       <c r="B238" s="4"/>
       <c r="C238" s="4" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D238" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F238" s="5" t="s">
         <v>110</v>
@@ -5954,10 +5966,10 @@
       <c r="A239" s="7"/>
       <c r="B239" s="4"/>
       <c r="C239" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F239" s="5" t="s">
         <v>110</v>
@@ -5967,31 +5979,31 @@
       <c r="A240" s="7"/>
       <c r="B240" s="4"/>
       <c r="C240" s="4" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D240" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F240" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="241" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A241" s="7"/>
       <c r="B241" s="4"/>
       <c r="C241" s="1" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D241" s="8" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F241" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="242" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A242" s="7" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B242" s="4" t="str">
         <f>'Mars Test Condition'!D57</f>
@@ -6024,10 +6036,10 @@
       <c r="A244" s="7"/>
       <c r="B244" s="4"/>
       <c r="C244" s="4" t="s">
-        <v>264</v>
+        <v>293</v>
       </c>
       <c r="D244" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F244" s="5" t="s">
         <v>110</v>
@@ -6037,10 +6049,10 @@
       <c r="A245" s="7"/>
       <c r="B245" s="4"/>
       <c r="C245" s="4" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D245" s="4" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="F245" s="5" t="s">
         <v>110</v>
@@ -6050,10 +6062,10 @@
       <c r="A246" s="7"/>
       <c r="B246" s="4"/>
       <c r="C246" s="4" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="F246" s="5" t="s">
         <v>118</v>
@@ -6061,7 +6073,7 @@
     </row>
     <row r="247" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A247" s="7" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B247" s="4" t="str">
         <f>'Mars Test Condition'!D58</f>
@@ -6094,10 +6106,10 @@
       <c r="A249" s="7"/>
       <c r="B249" s="4"/>
       <c r="C249" s="4" t="s">
-        <v>264</v>
+        <v>293</v>
       </c>
       <c r="D249" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F249" s="5" t="s">
         <v>110</v>
@@ -6107,10 +6119,10 @@
       <c r="A250" s="7"/>
       <c r="B250" s="4"/>
       <c r="C250" s="4" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D250" s="4" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="F250" s="5" t="s">
         <v>110</v>
@@ -6120,10 +6132,10 @@
       <c r="A251" s="7"/>
       <c r="B251" s="4"/>
       <c r="C251" s="4" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="F251" s="5" t="s">
         <v>118</v>
@@ -6131,7 +6143,7 @@
     </row>
     <row r="252" s="1" customFormat="1" ht="21" spans="1:6">
       <c r="A252" s="4" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B252" s="4" t="str">
         <f>'Mars Test Condition'!D59</f>
@@ -6164,10 +6176,10 @@
       <c r="A254" s="4"/>
       <c r="B254" s="4"/>
       <c r="C254" s="4" t="s">
-        <v>264</v>
+        <v>293</v>
       </c>
       <c r="D254" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F254" s="5" t="s">
         <v>110</v>
@@ -6177,10 +6189,10 @@
       <c r="A255" s="4"/>
       <c r="B255" s="4"/>
       <c r="C255" s="4" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="F255" s="5" t="s">
         <v>118</v>
@@ -6244,7 +6256,7 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" s="1" customFormat="1" ht="21" spans="3:3">
-      <c r="C275" s="10"/>
+      <c r="C275" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="116">

</xml_diff>